<commit_message>
actualizando tablas de bd3
</commit_message>
<xml_diff>
--- a/documentacion/EjemploDatosEnBd.xlsx
+++ b/documentacion/EjemploDatosEnBd.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MODULO USUARIO" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="103">
   <si>
     <t>LOGIN</t>
   </si>
@@ -153,13 +154,193 @@
   </si>
   <si>
     <t>FWEDFSF</t>
+  </si>
+  <si>
+    <t>registro_usuario</t>
+  </si>
+  <si>
+    <t>id_usuario</t>
+  </si>
+  <si>
+    <t>dni</t>
+  </si>
+  <si>
+    <t>nombres</t>
+  </si>
+  <si>
+    <t>ap_materno</t>
+  </si>
+  <si>
+    <t>telefono</t>
+  </si>
+  <si>
+    <t>fecha de nacimiento</t>
+  </si>
+  <si>
+    <t>ap_paterno</t>
+  </si>
+  <si>
+    <t>fecha de registro</t>
+  </si>
+  <si>
+    <t>celular</t>
+  </si>
+  <si>
+    <t>carnet de vacunacion</t>
+  </si>
+  <si>
+    <t>id_carnet</t>
+  </si>
+  <si>
+    <t>foto_carnet</t>
+  </si>
+  <si>
+    <t>productos</t>
+  </si>
+  <si>
+    <t>id_productos</t>
+  </si>
+  <si>
+    <t>tipo_producto</t>
+  </si>
+  <si>
+    <t>nombre_producto</t>
+  </si>
+  <si>
+    <t>iphone</t>
+  </si>
+  <si>
+    <t>precio_unitario_soles</t>
+  </si>
+  <si>
+    <t>tipo_usuario</t>
+  </si>
+  <si>
+    <t>pedrito</t>
+  </si>
+  <si>
+    <t>calle los pinos</t>
+  </si>
+  <si>
+    <t>cliente</t>
+  </si>
+  <si>
+    <t>provedor</t>
+  </si>
+  <si>
+    <t>id_provedor</t>
+  </si>
+  <si>
+    <t>fecha_ingreso</t>
+  </si>
+  <si>
+    <t>nombre_provedor</t>
+  </si>
+  <si>
+    <t>pedido_almacen</t>
+  </si>
+  <si>
+    <t>almacen</t>
+  </si>
+  <si>
+    <t>id_almacen</t>
+  </si>
+  <si>
+    <t>id_producto</t>
+  </si>
+  <si>
+    <t>cantidad_ingreso</t>
+  </si>
+  <si>
+    <t>cantidad_salida</t>
+  </si>
+  <si>
+    <t>fecha_salida</t>
+  </si>
+  <si>
+    <t>administrador_general</t>
+  </si>
+  <si>
+    <t>administrador_personal</t>
+  </si>
+  <si>
+    <t>fecha_registro</t>
+  </si>
+  <si>
+    <t>elec</t>
+  </si>
+  <si>
+    <t>apple</t>
+  </si>
+  <si>
+    <t>microsoft</t>
+  </si>
+  <si>
+    <t>id_tp_producto</t>
+  </si>
+  <si>
+    <t>laptop</t>
+  </si>
+  <si>
+    <t>nombre_tipo_producto</t>
+  </si>
+  <si>
+    <t>color_producto</t>
+  </si>
+  <si>
+    <t>id_color</t>
+  </si>
+  <si>
+    <t>nombre_color</t>
+  </si>
+  <si>
+    <t>rojo</t>
+  </si>
+  <si>
+    <t>verde</t>
+  </si>
+  <si>
+    <t>amarillo</t>
+  </si>
+  <si>
+    <t>azul</t>
+  </si>
+  <si>
+    <t>color_id</t>
+  </si>
+  <si>
+    <t>cantidad_actual</t>
+  </si>
+  <si>
+    <t>id_pedido</t>
+  </si>
+  <si>
+    <t>cantidad_pedido</t>
+  </si>
+  <si>
+    <t>fecha_pedido</t>
+  </si>
+  <si>
+    <t>tipo_peso</t>
+  </si>
+  <si>
+    <t>almacen producto</t>
+  </si>
+  <si>
+    <t>id_almacen_producto</t>
+  </si>
+  <si>
+    <t>cantidad_Actual</t>
+  </si>
+  <si>
+    <t>stock</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,8 +355,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,6 +397,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -286,12 +504,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -325,7 +544,16 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,26 +851,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="G4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="8"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="G4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="9"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -665,7 +893,7 @@
       <c r="J5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="K5" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -729,17 +957,17 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="11"/>
-      <c r="H16" s="12" t="s">
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="12"/>
+      <c r="H16" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="I16" s="13"/>
+      <c r="I16" s="14"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
@@ -925,4 +1153,628 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:S42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="21.28515625" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" customWidth="1"/>
+    <col min="12" max="12" width="18" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" customWidth="1"/>
+    <col min="16" max="16" width="15.140625" customWidth="1"/>
+    <col min="18" max="18" width="21.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="S3" s="17"/>
+    </row>
+    <row r="4" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q4" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="R4" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="S4" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" t="s">
+        <v>48</v>
+      </c>
+      <c r="K5" t="s">
+        <v>49</v>
+      </c>
+      <c r="L5" t="s">
+        <v>51</v>
+      </c>
+      <c r="M5" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
+    </row>
+    <row r="6" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>312312</v>
+      </c>
+      <c r="E6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I6">
+        <v>9878978978</v>
+      </c>
+      <c r="J6">
+        <v>343434</v>
+      </c>
+      <c r="K6" s="18">
+        <v>701</v>
+      </c>
+      <c r="L6" s="18">
+        <v>701</v>
+      </c>
+      <c r="M6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>3213123</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7">
+        <v>987978978</v>
+      </c>
+      <c r="J7">
+        <v>434344</v>
+      </c>
+      <c r="K7" s="18">
+        <v>701</v>
+      </c>
+      <c r="L7" s="18">
+        <v>701</v>
+      </c>
+      <c r="M7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>32131</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I8">
+        <v>9789789</v>
+      </c>
+      <c r="J8">
+        <v>343434</v>
+      </c>
+      <c r="K8" s="18">
+        <v>701</v>
+      </c>
+      <c r="L8" s="18">
+        <v>701</v>
+      </c>
+      <c r="M8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="L15" s="20"/>
+      <c r="M15" s="20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>56</v>
+      </c>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="L16" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="M16" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="G17" t="s">
+        <v>61</v>
+      </c>
+      <c r="H17" t="s">
+        <v>102</v>
+      </c>
+      <c r="I17" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="J17" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="L17" s="20">
+        <v>1</v>
+      </c>
+      <c r="M17" s="20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>23333</v>
+      </c>
+      <c r="H18">
+        <v>200</v>
+      </c>
+      <c r="I18" s="19">
+        <v>1</v>
+      </c>
+      <c r="J18" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="L18" s="20">
+        <v>2</v>
+      </c>
+      <c r="M18" s="20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="I19" s="19">
+        <v>2</v>
+      </c>
+      <c r="J19" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="L19" s="20">
+        <v>3</v>
+      </c>
+      <c r="M19" s="20" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="L20" s="20">
+        <v>4</v>
+      </c>
+      <c r="M20" s="20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" s="18">
+        <v>701</v>
+      </c>
+      <c r="E26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27" s="18">
+        <v>701</v>
+      </c>
+      <c r="E27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28" s="18">
+        <v>701</v>
+      </c>
+      <c r="E28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="M30" s="21"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="21"/>
+    </row>
+    <row r="31" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C31" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="F31" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="G31" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="H31" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="I31" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="J31" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="K31" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="L31" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="M31" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="N31" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="O31" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="P31" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C32" s="23">
+        <v>1</v>
+      </c>
+      <c r="D32" s="23">
+        <v>1</v>
+      </c>
+      <c r="E32" s="23">
+        <v>2333</v>
+      </c>
+      <c r="F32" s="23">
+        <v>1122</v>
+      </c>
+      <c r="G32" s="23">
+        <v>1</v>
+      </c>
+      <c r="H32" s="24">
+        <v>701</v>
+      </c>
+      <c r="I32" s="24">
+        <v>701</v>
+      </c>
+      <c r="J32" s="26">
+        <v>200</v>
+      </c>
+      <c r="K32" s="21">
+        <v>1</v>
+      </c>
+      <c r="L32" s="21">
+        <v>1</v>
+      </c>
+      <c r="M32" s="21">
+        <v>1</v>
+      </c>
+      <c r="N32" s="21">
+        <v>233</v>
+      </c>
+      <c r="O32" s="22">
+        <v>701</v>
+      </c>
+      <c r="P32" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C33" s="23">
+        <v>2</v>
+      </c>
+      <c r="D33" s="23">
+        <v>1</v>
+      </c>
+      <c r="E33" s="23">
+        <v>233</v>
+      </c>
+      <c r="F33" s="23">
+        <v>122</v>
+      </c>
+      <c r="G33" s="23">
+        <v>1</v>
+      </c>
+      <c r="H33" s="24">
+        <v>701</v>
+      </c>
+      <c r="I33" s="24">
+        <v>701</v>
+      </c>
+      <c r="J33" s="26"/>
+      <c r="K33" s="21">
+        <v>2</v>
+      </c>
+      <c r="L33" s="21">
+        <v>1</v>
+      </c>
+      <c r="M33" s="21">
+        <v>1</v>
+      </c>
+      <c r="N33" s="21">
+        <v>233</v>
+      </c>
+      <c r="O33" s="22">
+        <v>701</v>
+      </c>
+      <c r="P33" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C34" s="23">
+        <v>3</v>
+      </c>
+      <c r="D34" s="23">
+        <v>1</v>
+      </c>
+      <c r="E34" s="23">
+        <v>233</v>
+      </c>
+      <c r="F34" s="23">
+        <v>11</v>
+      </c>
+      <c r="G34" s="23">
+        <v>1</v>
+      </c>
+      <c r="H34" s="24">
+        <v>701</v>
+      </c>
+      <c r="I34" s="24">
+        <v>701</v>
+      </c>
+      <c r="J34" s="26"/>
+      <c r="K34" s="21">
+        <v>3</v>
+      </c>
+      <c r="L34" s="21">
+        <v>2</v>
+      </c>
+      <c r="M34" s="21">
+        <v>2</v>
+      </c>
+      <c r="N34" s="21">
+        <v>233</v>
+      </c>
+      <c r="O34" s="22">
+        <v>701</v>
+      </c>
+      <c r="P34" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C35" s="23">
+        <v>4</v>
+      </c>
+      <c r="D35" s="23">
+        <v>2</v>
+      </c>
+      <c r="E35" s="23">
+        <v>2333</v>
+      </c>
+      <c r="F35" s="23">
+        <v>112</v>
+      </c>
+      <c r="G35" s="23">
+        <v>2</v>
+      </c>
+      <c r="H35" s="24">
+        <v>701</v>
+      </c>
+      <c r="I35" s="24">
+        <v>701</v>
+      </c>
+      <c r="J35" s="26"/>
+      <c r="K35" s="21"/>
+      <c r="L35" s="21"/>
+      <c r="M35" s="21"/>
+      <c r="N35" s="21"/>
+      <c r="O35" s="22">
+        <v>701</v>
+      </c>
+      <c r="P35" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C36" s="23">
+        <v>5</v>
+      </c>
+      <c r="D36" s="23">
+        <v>1</v>
+      </c>
+      <c r="E36" s="23">
+        <v>23333</v>
+      </c>
+      <c r="F36" s="23">
+        <v>112</v>
+      </c>
+      <c r="G36" s="23">
+        <v>1</v>
+      </c>
+      <c r="H36" s="24">
+        <v>701</v>
+      </c>
+      <c r="I36" s="24">
+        <v>701</v>
+      </c>
+      <c r="J36" s="26"/>
+      <c r="K36" s="21"/>
+      <c r="L36" s="21"/>
+      <c r="M36" s="21"/>
+      <c r="N36" s="21"/>
+      <c r="O36" s="21"/>
+    </row>
+    <row r="37" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="H40" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>100</v>
+      </c>
+      <c r="H41" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>6</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>12</v>
+      </c>
+      <c r="F42">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
agregando productos a backend
</commit_message>
<xml_diff>
--- a/documentacion/EjemploDatosEnBd.xlsx
+++ b/documentacion/EjemploDatosEnBd.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="122">
   <si>
     <t>LOGIN</t>
   </si>
@@ -321,9 +321,6 @@
     <t>fecha_pedido</t>
   </si>
   <si>
-    <t>tipo_peso</t>
-  </si>
-  <si>
     <t>almacen producto</t>
   </si>
   <si>
@@ -334,13 +331,73 @@
   </si>
   <si>
     <t>stock</t>
+  </si>
+  <si>
+    <t>extras</t>
+  </si>
+  <si>
+    <t>estado_usuario</t>
+  </si>
+  <si>
+    <t>activo</t>
+  </si>
+  <si>
+    <t>inactivo</t>
+  </si>
+  <si>
+    <t>Polos</t>
+  </si>
+  <si>
+    <t>FECHA_VENTA</t>
+  </si>
+  <si>
+    <t>TOTAL($)</t>
+  </si>
+  <si>
+    <t>$=SOLES</t>
+  </si>
+  <si>
+    <t>ID_PRODUCTO</t>
+  </si>
+  <si>
+    <t>CANTIDAD</t>
+  </si>
+  <si>
+    <t>COMPRA_PRODUCTO-USUARIO</t>
+  </si>
+  <si>
+    <t>DETALLE_COMPRA_PRODUCTO-USUARIO</t>
+  </si>
+  <si>
+    <t>ID_VENTA(PK)</t>
+  </si>
+  <si>
+    <t>ID_USUARIO(PK)(FK)</t>
+  </si>
+  <si>
+    <t>13/3/2022</t>
+  </si>
+  <si>
+    <t>IGV?</t>
+  </si>
+  <si>
+    <t>tipo_CATEGORIA</t>
+  </si>
+  <si>
+    <t>MARCA</t>
+  </si>
+  <si>
+    <t>idMarca</t>
+  </si>
+  <si>
+    <t>nombreMarca</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,8 +419,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="0"/>
+      <name val="Algerian"/>
+      <family val="5"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Algerian"/>
+      <family val="5"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Algerian"/>
+      <family val="5"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Algerian"/>
+      <family val="5"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Algerian"/>
+      <family val="5"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -430,8 +524,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -500,60 +618,120 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -851,26 +1029,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="G4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="9"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="G4" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="17"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -957,17 +1135,17 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="12"/>
-      <c r="H16" s="13" t="s">
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="20"/>
+      <c r="H16" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="I16" s="14"/>
+      <c r="I16" s="22"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
@@ -1159,8 +1337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,27 +1357,31 @@
     <col min="14" max="14" width="16.42578125" customWidth="1"/>
     <col min="15" max="15" width="14.7109375" customWidth="1"/>
     <col min="16" max="16" width="15.140625" customWidth="1"/>
+    <col min="17" max="17" width="15.85546875" customWidth="1"/>
     <col min="18" max="18" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17" t="s">
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="S3" s="17"/>
+      <c r="S3" s="6"/>
     </row>
     <row r="4" spans="3:19" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
         <v>43</v>
       </c>
-      <c r="Q4" s="17" t="s">
+      <c r="N4" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q4" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="R4" s="17" t="s">
+      <c r="R4" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="S4" s="17" t="s">
+      <c r="S4" s="6" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1237,9 +1419,12 @@
       <c r="M5" t="s">
         <v>62</v>
       </c>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
+      <c r="N5" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
     </row>
     <row r="6" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C6">
@@ -1260,14 +1445,17 @@
       <c r="J6">
         <v>343434</v>
       </c>
-      <c r="K6" s="18">
-        <v>701</v>
-      </c>
-      <c r="L6" s="18">
+      <c r="K6" s="7">
+        <v>701</v>
+      </c>
+      <c r="L6" s="7">
         <v>701</v>
       </c>
       <c r="M6" t="s">
         <v>65</v>
+      </c>
+      <c r="N6" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="3:19" x14ac:dyDescent="0.25">
@@ -1289,14 +1477,17 @@
       <c r="J7">
         <v>434344</v>
       </c>
-      <c r="K7" s="18">
-        <v>701</v>
-      </c>
-      <c r="L7" s="18">
+      <c r="K7" s="7">
+        <v>701</v>
+      </c>
+      <c r="L7" s="7">
         <v>701</v>
       </c>
       <c r="M7" t="s">
         <v>77</v>
+      </c>
+      <c r="N7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="3:19" x14ac:dyDescent="0.25">
@@ -1318,132 +1509,250 @@
       <c r="J8">
         <v>343434</v>
       </c>
-      <c r="K8" s="18">
-        <v>701</v>
-      </c>
-      <c r="L8" s="18">
+      <c r="K8" s="7">
+        <v>701</v>
+      </c>
+      <c r="L8" s="7">
         <v>701</v>
       </c>
       <c r="M8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="L15" s="20"/>
-      <c r="M15" s="20" t="s">
+    <row r="11" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="E11" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="F11" s="45"/>
+      <c r="R11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="E12" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="F12" s="43" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+    </row>
+    <row r="15" spans="3:19" ht="21.75" x14ac:dyDescent="0.35">
+      <c r="L15" s="40" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="16" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="E16" t="s">
+      <c r="M15" s="41"/>
+      <c r="O15" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="P15" s="39"/>
+      <c r="Q15" s="39"/>
+      <c r="R15" s="39"/>
+    </row>
+    <row r="16" spans="3:19" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C16" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17" t="s">
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="J16" s="31"/>
+      <c r="L16" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="M16" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="O16" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="P16" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q16" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="R16" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="S16" s="42" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C17" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="L16" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="M16" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="E17" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="F17" s="20" t="s">
+      <c r="F17" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="H17" t="s">
-        <v>102</v>
-      </c>
-      <c r="I17" s="19" t="s">
+      <c r="H17" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="I17" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="J17" s="19" t="s">
+      <c r="J17" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="L17" s="20">
-        <v>1</v>
-      </c>
-      <c r="M17" s="20" t="s">
+      <c r="L17" s="32">
+        <v>1</v>
+      </c>
+      <c r="M17" s="32" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="O17" s="34">
+        <v>1</v>
+      </c>
+      <c r="P17" s="35">
+        <v>44898</v>
+      </c>
+      <c r="Q17" s="34">
+        <v>600</v>
+      </c>
+      <c r="R17" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C18" s="25">
+        <v>1</v>
+      </c>
+      <c r="D18" s="25">
+        <v>1</v>
+      </c>
+      <c r="E18" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
+      <c r="F18" s="25">
+        <v>1</v>
+      </c>
+      <c r="G18" s="25">
         <v>23333</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="25">
         <v>200</v>
       </c>
-      <c r="I18" s="19">
-        <v>1</v>
-      </c>
-      <c r="J18" s="19" t="s">
+      <c r="I18" s="29">
+        <v>1</v>
+      </c>
+      <c r="J18" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="L18" s="20">
+      <c r="L18" s="32">
         <v>2</v>
       </c>
-      <c r="M18" s="20" t="s">
+      <c r="M18" s="32" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="I19" s="19">
+      <c r="O18" s="34">
         <v>2</v>
       </c>
-      <c r="J19" s="19" t="s">
+      <c r="P18" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q18" s="34">
+        <v>400</v>
+      </c>
+      <c r="R18" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="29">
+        <v>2</v>
+      </c>
+      <c r="J19" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="L19" s="20">
+      <c r="L19" s="32">
         <v>3</v>
       </c>
-      <c r="M19" s="20" t="s">
+      <c r="M19" s="32" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="L20" s="20">
+      <c r="O19" s="34"/>
+      <c r="P19" s="34"/>
+      <c r="Q19" s="34"/>
+      <c r="R19" s="34"/>
+    </row>
+    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="29">
+        <v>3</v>
+      </c>
+      <c r="J20" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="L20" s="32">
         <v>4</v>
       </c>
-      <c r="M20" s="20" t="s">
+      <c r="M20" s="32" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="L21" s="33"/>
+      <c r="M21" s="33"/>
+    </row>
+    <row r="23" spans="3:18" ht="21.75" x14ac:dyDescent="0.35">
+      <c r="O23" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="P23" s="38"/>
+      <c r="Q23" s="38"/>
+      <c r="R23" s="38"/>
+    </row>
+    <row r="24" spans="3:18" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="O24" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="P24" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q24" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="R24" s="37"/>
+    </row>
+    <row r="25" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>67</v>
       </c>
@@ -1453,293 +1762,327 @@
       <c r="E25" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="O25" s="36">
+        <v>1</v>
+      </c>
+      <c r="P25" s="36">
+        <v>2</v>
+      </c>
+      <c r="Q25" s="36">
+        <v>20</v>
+      </c>
+      <c r="R25" s="37"/>
+    </row>
+    <row r="26" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" s="18">
+      <c r="D26" s="7">
         <v>701</v>
       </c>
       <c r="E26" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="O26" s="36">
+        <v>1</v>
+      </c>
+      <c r="P26" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="36">
+        <v>30</v>
+      </c>
+      <c r="R26" s="37"/>
+    </row>
+    <row r="27" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>2</v>
       </c>
-      <c r="D27" s="18">
+      <c r="D27" s="7">
         <v>701</v>
       </c>
       <c r="E27" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="O27" s="36">
+        <v>1</v>
+      </c>
+      <c r="P27" s="36">
+        <v>3</v>
+      </c>
+      <c r="Q27" s="36">
+        <v>5</v>
+      </c>
+      <c r="R27" s="37"/>
+    </row>
+    <row r="28" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>3</v>
       </c>
-      <c r="D28" s="18">
+      <c r="D28" s="7">
         <v>701</v>
       </c>
       <c r="E28" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="30" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23" t="s">
+      <c r="O28" s="37"/>
+      <c r="P28" s="37"/>
+      <c r="Q28" s="37"/>
+      <c r="R28" s="37"/>
+    </row>
+    <row r="30" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="21" t="s">
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="M30" s="21"/>
-      <c r="N30" s="21"/>
-      <c r="O30" s="21"/>
-    </row>
-    <row r="31" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C31" s="23" t="s">
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+    </row>
+    <row r="31" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C31" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D31" s="23" t="s">
+      <c r="D31" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="E31" s="23" t="s">
+      <c r="E31" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="F31" s="23" t="s">
+      <c r="F31" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="G31" s="23" t="s">
+      <c r="G31" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="H31" s="23" t="s">
+      <c r="H31" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="I31" s="23" t="s">
+      <c r="I31" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="J31" s="26" t="s">
+      <c r="J31" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="K31" s="21" t="s">
+      <c r="K31" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="L31" s="21" t="s">
+      <c r="L31" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="M31" s="21" t="s">
+      <c r="M31" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="N31" s="21" t="s">
+      <c r="N31" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="O31" s="21" t="s">
+      <c r="O31" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="P31" s="25" t="s">
+      <c r="P31" s="12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C32" s="23">
-        <v>1</v>
-      </c>
-      <c r="D32" s="23">
-        <v>1</v>
-      </c>
-      <c r="E32" s="23">
+    <row r="32" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C32" s="10">
+        <v>1</v>
+      </c>
+      <c r="D32" s="10">
+        <v>1</v>
+      </c>
+      <c r="E32" s="10">
         <v>2333</v>
       </c>
-      <c r="F32" s="23">
+      <c r="F32" s="10">
         <v>1122</v>
       </c>
-      <c r="G32" s="23">
-        <v>1</v>
-      </c>
-      <c r="H32" s="24">
-        <v>701</v>
-      </c>
-      <c r="I32" s="24">
-        <v>701</v>
-      </c>
-      <c r="J32" s="26">
+      <c r="G32" s="10">
+        <v>1</v>
+      </c>
+      <c r="H32" s="11">
+        <v>701</v>
+      </c>
+      <c r="I32" s="11">
+        <v>701</v>
+      </c>
+      <c r="J32" s="13">
         <v>200</v>
       </c>
-      <c r="K32" s="21">
-        <v>1</v>
-      </c>
-      <c r="L32" s="21">
-        <v>1</v>
-      </c>
-      <c r="M32" s="21">
-        <v>1</v>
-      </c>
-      <c r="N32" s="21">
+      <c r="K32" s="8">
+        <v>1</v>
+      </c>
+      <c r="L32" s="8">
+        <v>1</v>
+      </c>
+      <c r="M32" s="8">
+        <v>1</v>
+      </c>
+      <c r="N32" s="8">
         <v>233</v>
       </c>
-      <c r="O32" s="22">
-        <v>701</v>
-      </c>
-      <c r="P32" s="25">
+      <c r="O32" s="9">
+        <v>701</v>
+      </c>
+      <c r="P32" s="12">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C33" s="23">
+      <c r="C33" s="10">
         <v>2</v>
       </c>
-      <c r="D33" s="23">
-        <v>1</v>
-      </c>
-      <c r="E33" s="23">
+      <c r="D33" s="10">
+        <v>1</v>
+      </c>
+      <c r="E33" s="10">
         <v>233</v>
       </c>
-      <c r="F33" s="23">
+      <c r="F33" s="10">
         <v>122</v>
       </c>
-      <c r="G33" s="23">
-        <v>1</v>
-      </c>
-      <c r="H33" s="24">
-        <v>701</v>
-      </c>
-      <c r="I33" s="24">
-        <v>701</v>
-      </c>
-      <c r="J33" s="26"/>
-      <c r="K33" s="21">
+      <c r="G33" s="10">
+        <v>1</v>
+      </c>
+      <c r="H33" s="11">
+        <v>701</v>
+      </c>
+      <c r="I33" s="11">
+        <v>701</v>
+      </c>
+      <c r="J33" s="13"/>
+      <c r="K33" s="8">
         <v>2</v>
       </c>
-      <c r="L33" s="21">
-        <v>1</v>
-      </c>
-      <c r="M33" s="21">
-        <v>1</v>
-      </c>
-      <c r="N33" s="21">
+      <c r="L33" s="8">
+        <v>1</v>
+      </c>
+      <c r="M33" s="8">
+        <v>1</v>
+      </c>
+      <c r="N33" s="8">
         <v>233</v>
       </c>
-      <c r="O33" s="22">
-        <v>701</v>
-      </c>
-      <c r="P33" s="25">
+      <c r="O33" s="9">
+        <v>701</v>
+      </c>
+      <c r="P33" s="12">
         <v>2</v>
       </c>
     </row>
     <row r="34" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C34" s="23">
+      <c r="C34" s="10">
         <v>3</v>
       </c>
-      <c r="D34" s="23">
-        <v>1</v>
-      </c>
-      <c r="E34" s="23">
+      <c r="D34" s="10">
+        <v>1</v>
+      </c>
+      <c r="E34" s="10">
         <v>233</v>
       </c>
-      <c r="F34" s="23">
+      <c r="F34" s="10">
         <v>11</v>
       </c>
-      <c r="G34" s="23">
-        <v>1</v>
-      </c>
-      <c r="H34" s="24">
-        <v>701</v>
-      </c>
-      <c r="I34" s="24">
-        <v>701</v>
-      </c>
-      <c r="J34" s="26"/>
-      <c r="K34" s="21">
+      <c r="G34" s="10">
+        <v>1</v>
+      </c>
+      <c r="H34" s="11">
+        <v>701</v>
+      </c>
+      <c r="I34" s="11">
+        <v>701</v>
+      </c>
+      <c r="J34" s="13"/>
+      <c r="K34" s="8">
         <v>3</v>
       </c>
-      <c r="L34" s="21">
+      <c r="L34" s="8">
         <v>2</v>
       </c>
-      <c r="M34" s="21">
+      <c r="M34" s="8">
         <v>2</v>
       </c>
-      <c r="N34" s="21">
+      <c r="N34" s="8">
         <v>233</v>
       </c>
-      <c r="O34" s="22">
-        <v>701</v>
-      </c>
-      <c r="P34" s="25">
+      <c r="O34" s="9">
+        <v>701</v>
+      </c>
+      <c r="P34" s="12">
         <v>2</v>
       </c>
     </row>
     <row r="35" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C35" s="23">
+      <c r="C35" s="10">
         <v>4</v>
       </c>
-      <c r="D35" s="23">
+      <c r="D35" s="10">
         <v>2</v>
       </c>
-      <c r="E35" s="23">
+      <c r="E35" s="10">
         <v>2333</v>
       </c>
-      <c r="F35" s="23">
+      <c r="F35" s="10">
         <v>112</v>
       </c>
-      <c r="G35" s="23">
+      <c r="G35" s="10">
         <v>2</v>
       </c>
-      <c r="H35" s="24">
-        <v>701</v>
-      </c>
-      <c r="I35" s="24">
-        <v>701</v>
-      </c>
-      <c r="J35" s="26"/>
-      <c r="K35" s="21"/>
-      <c r="L35" s="21"/>
-      <c r="M35" s="21"/>
-      <c r="N35" s="21"/>
-      <c r="O35" s="22">
-        <v>701</v>
-      </c>
-      <c r="P35" s="25">
+      <c r="H35" s="11">
+        <v>701</v>
+      </c>
+      <c r="I35" s="11">
+        <v>701</v>
+      </c>
+      <c r="J35" s="13"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="9">
+        <v>701</v>
+      </c>
+      <c r="P35" s="12">
         <v>3</v>
       </c>
     </row>
     <row r="36" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C36" s="23">
+      <c r="C36" s="10">
         <v>5</v>
       </c>
-      <c r="D36" s="23">
-        <v>1</v>
-      </c>
-      <c r="E36" s="23">
+      <c r="D36" s="10">
+        <v>1</v>
+      </c>
+      <c r="E36" s="10">
         <v>23333</v>
       </c>
-      <c r="F36" s="23">
+      <c r="F36" s="10">
         <v>112</v>
       </c>
-      <c r="G36" s="23">
-        <v>1</v>
-      </c>
-      <c r="H36" s="24">
-        <v>701</v>
-      </c>
-      <c r="I36" s="24">
-        <v>701</v>
-      </c>
-      <c r="J36" s="26"/>
-      <c r="K36" s="21"/>
-      <c r="L36" s="21"/>
-      <c r="M36" s="21"/>
-      <c r="N36" s="21"/>
-      <c r="O36" s="21"/>
+      <c r="G36" s="10">
+        <v>1</v>
+      </c>
+      <c r="H36" s="11">
+        <v>701</v>
+      </c>
+      <c r="I36" s="11">
+        <v>701</v>
+      </c>
+      <c r="J36" s="13"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
     </row>
     <row r="37" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D37">
@@ -1748,15 +2091,15 @@
     </row>
     <row r="40" spans="3:16" x14ac:dyDescent="0.25">
       <c r="H40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="3:16" x14ac:dyDescent="0.25">
       <c r="G41" t="s">
+        <v>99</v>
+      </c>
+      <c r="H41" t="s">
         <v>100</v>
-      </c>
-      <c r="H41" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="42" spans="3:16" x14ac:dyDescent="0.25">
@@ -1774,6 +2117,14 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="O23:R23"/>
+    <mergeCell ref="O15:R15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
pequeños cambios 1 de octubre
</commit_message>
<xml_diff>
--- a/documentacion/EjemploDatosEnBd.xlsx
+++ b/documentacion/EjemploDatosEnBd.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="144">
   <si>
     <t>LOGIN</t>
   </si>
@@ -451,6 +451,12 @@
   </si>
   <si>
     <t>hallowin</t>
+  </si>
+  <si>
+    <t>imagenProducto</t>
+  </si>
+  <si>
+    <t>fdsfds.pnj</t>
   </si>
 </sst>
 </file>
@@ -745,7 +751,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -777,93 +783,60 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -873,6 +846,40 @@
     <xf numFmtId="0" fontId="11" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1170,26 +1177,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5" customHeight="1">
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="G4" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="26"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="G4" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="32"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
@@ -1276,17 +1283,17 @@
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="29"/>
-      <c r="H16" s="30" t="s">
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="35"/>
+      <c r="H16" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="I16" s="31"/>
+      <c r="I16" s="37"/>
     </row>
     <row r="17" spans="2:12">
       <c r="B17" s="3" t="s">
@@ -1476,14 +1483,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:AD42"/>
+  <dimension ref="B3:AD42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="X30" sqref="X30"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="7.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
     <col min="3" max="3" width="13.140625" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" customWidth="1"/>
@@ -1506,25 +1515,25 @@
     <col min="29" max="29" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:30" ht="21.75">
+    <row r="3" spans="2:30" ht="21.75">
       <c r="Q3" s="6"/>
       <c r="R3" s="6" t="s">
         <v>53</v>
       </c>
       <c r="S3" s="6"/>
-      <c r="X3" s="51" t="s">
+      <c r="X3" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="Y3" s="52"/>
+      <c r="Y3" s="44"/>
       <c r="AB3" s="15"/>
-      <c r="AC3" s="53" t="s">
+      <c r="AC3" s="26" t="s">
         <v>130</v>
       </c>
       <c r="AD3" s="15" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="3:30">
+    <row r="4" spans="2:30">
       <c r="E4" t="s">
         <v>43</v>
       </c>
@@ -1540,10 +1549,10 @@
       <c r="S4" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="X4" s="50">
-        <v>1</v>
-      </c>
-      <c r="Y4" s="50">
+      <c r="X4" s="25">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="25">
         <v>24</v>
       </c>
       <c r="AB4" s="15">
@@ -1556,7 +1565,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="3:30">
+    <row r="5" spans="2:30">
       <c r="C5" t="s">
         <v>44</v>
       </c>
@@ -1596,10 +1605,10 @@
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
       <c r="S5" s="6"/>
-      <c r="X5" s="50">
+      <c r="X5" s="25">
         <v>2</v>
       </c>
-      <c r="Y5" s="50">
+      <c r="Y5" s="25">
         <v>65</v>
       </c>
       <c r="AB5" s="15">
@@ -1612,7 +1621,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="3:30">
+    <row r="6" spans="2:30">
       <c r="C6">
         <v>1</v>
       </c>
@@ -1643,10 +1652,10 @@
       <c r="N6" t="s">
         <v>104</v>
       </c>
-      <c r="X6" s="50">
+      <c r="X6" s="25">
         <v>3</v>
       </c>
-      <c r="Y6" s="50">
+      <c r="Y6" s="25">
         <v>43</v>
       </c>
       <c r="AB6" s="15">
@@ -1659,7 +1668,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="3:30">
+    <row r="7" spans="2:30">
       <c r="C7">
         <v>2</v>
       </c>
@@ -1690,13 +1699,13 @@
       <c r="N7" t="s">
         <v>105</v>
       </c>
-      <c r="X7" s="50"/>
-      <c r="Y7" s="50"/>
+      <c r="X7" s="25"/>
+      <c r="Y7" s="25"/>
       <c r="AB7" s="15"/>
       <c r="AC7" s="15"/>
       <c r="AD7" s="15"/>
     </row>
-    <row r="8" spans="3:30">
+    <row r="8" spans="2:30">
       <c r="C8">
         <v>3</v>
       </c>
@@ -1725,19 +1734,19 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="3:30">
-      <c r="E10" s="47"/>
-    </row>
-    <row r="11" spans="3:30">
-      <c r="E11" s="36" t="s">
+    <row r="10" spans="2:30">
+      <c r="E10" s="23"/>
+    </row>
+    <row r="11" spans="2:30">
+      <c r="E11" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="F11" s="37"/>
+      <c r="F11" s="51"/>
       <c r="R11" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="3:30">
+    <row r="12" spans="2:30">
       <c r="E12" s="22" t="s">
         <v>119</v>
       </c>
@@ -1745,35 +1754,36 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="3:30">
+    <row r="13" spans="2:30">
       <c r="E13" s="22"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="15" spans="3:30" ht="21.75">
-      <c r="L15" s="43" t="s">
+    <row r="15" spans="2:30" ht="21.75">
+      <c r="L15" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="M15" s="44"/>
-      <c r="O15" s="46" t="s">
+      <c r="M15" s="58"/>
+      <c r="O15" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="P15" s="46"/>
-      <c r="Q15" s="46"/>
-      <c r="R15" s="46"/>
-    </row>
-    <row r="16" spans="3:30" ht="34.5">
-      <c r="C16" s="38" t="s">
+      <c r="P15" s="41"/>
+      <c r="Q15" s="41"/>
+      <c r="R15" s="41"/>
+    </row>
+    <row r="16" spans="2:30" ht="34.5">
+      <c r="B16" s="59"/>
+      <c r="C16" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="41" t="s">
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="55" t="s">
         <v>117</v>
       </c>
-      <c r="J16" s="42"/>
+      <c r="J16" s="56"/>
       <c r="L16" s="15" t="s">
         <v>87</v>
       </c>
@@ -1795,15 +1805,18 @@
       <c r="S16" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="X16" s="56" t="s">
+      <c r="X16" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="Y16" s="57"/>
-      <c r="Z16" s="57"/>
-      <c r="AA16" s="57"/>
-      <c r="AB16" s="58"/>
-    </row>
-    <row r="17" spans="3:28">
+      <c r="Y16" s="46"/>
+      <c r="Z16" s="46"/>
+      <c r="AA16" s="46"/>
+      <c r="AB16" s="47"/>
+    </row>
+    <row r="17" spans="2:28">
+      <c r="B17" s="13" t="s">
+        <v>142</v>
+      </c>
       <c r="C17" s="13" t="s">
         <v>57</v>
       </c>
@@ -1846,23 +1859,26 @@
       <c r="R17" s="17">
         <v>1</v>
       </c>
-      <c r="X17" s="54" t="s">
+      <c r="X17" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="Y17" s="54" t="s">
+      <c r="Y17" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="Z17" s="54" t="s">
+      <c r="Z17" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="AA17" s="54" t="s">
+      <c r="AA17" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="AB17" s="54" t="s">
+      <c r="AB17" s="27" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="3:28">
+    <row r="18" spans="2:28">
+      <c r="B18" s="13" t="s">
+        <v>143</v>
+      </c>
       <c r="C18" s="13">
         <v>1</v>
       </c>
@@ -1905,23 +1921,24 @@
       <c r="R18" s="17">
         <v>1</v>
       </c>
-      <c r="X18" s="54">
-        <v>1</v>
-      </c>
-      <c r="Y18" s="54">
+      <c r="X18" s="27">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="27">
         <v>2</v>
       </c>
-      <c r="Z18" s="55">
+      <c r="Z18" s="28">
         <v>0.1</v>
       </c>
-      <c r="AA18" s="54">
-        <v>1</v>
-      </c>
-      <c r="AB18" s="54" t="s">
+      <c r="AA18" s="27">
+        <v>1</v>
+      </c>
+      <c r="AB18" s="27" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="3:28">
+    <row r="19" spans="2:28">
+      <c r="B19" s="59"/>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
       <c r="E19" s="13"/>
@@ -1944,13 +1961,14 @@
       <c r="P19" s="17"/>
       <c r="Q19" s="17"/>
       <c r="R19" s="17"/>
-      <c r="X19" s="54"/>
-      <c r="Y19" s="54"/>
-      <c r="Z19" s="54"/>
-      <c r="AA19" s="54"/>
-      <c r="AB19" s="54"/>
-    </row>
-    <row r="20" spans="3:28">
+      <c r="X19" s="27"/>
+      <c r="Y19" s="27"/>
+      <c r="Z19" s="27"/>
+      <c r="AA19" s="27"/>
+      <c r="AB19" s="27"/>
+    </row>
+    <row r="20" spans="2:28">
+      <c r="B20" s="59"/>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
       <c r="E20" s="13"/>
@@ -1969,13 +1987,14 @@
       <c r="M20" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="X20" s="54"/>
-      <c r="Y20" s="54"/>
-      <c r="Z20" s="54"/>
-      <c r="AA20" s="54"/>
-      <c r="AB20" s="54"/>
-    </row>
-    <row r="21" spans="3:28">
+      <c r="X20" s="27"/>
+      <c r="Y20" s="27"/>
+      <c r="Z20" s="27"/>
+      <c r="AA20" s="27"/>
+      <c r="AB20" s="27"/>
+    </row>
+    <row r="21" spans="2:28">
+      <c r="B21" s="59"/>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
@@ -1984,38 +2003,38 @@
       <c r="H21" s="13"/>
       <c r="L21" s="16"/>
       <c r="M21" s="16"/>
-      <c r="X21" s="54"/>
-      <c r="Y21" s="54"/>
-      <c r="Z21" s="54"/>
-      <c r="AA21" s="54"/>
-      <c r="AB21" s="54"/>
-    </row>
-    <row r="22" spans="3:28">
-      <c r="X22" s="54"/>
-      <c r="Y22" s="54"/>
-      <c r="Z22" s="54"/>
-      <c r="AA22" s="54"/>
-      <c r="AB22" s="54"/>
-    </row>
-    <row r="23" spans="3:28" ht="21.75">
-      <c r="O23" s="45" t="s">
+      <c r="X21" s="27"/>
+      <c r="Y21" s="27"/>
+      <c r="Z21" s="27"/>
+      <c r="AA21" s="27"/>
+      <c r="AB21" s="27"/>
+    </row>
+    <row r="22" spans="2:28">
+      <c r="X22" s="27"/>
+      <c r="Y22" s="27"/>
+      <c r="Z22" s="27"/>
+      <c r="AA22" s="27"/>
+      <c r="AB22" s="27"/>
+    </row>
+    <row r="23" spans="2:28" ht="21.75">
+      <c r="O23" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="P23" s="45"/>
-      <c r="Q23" s="45"/>
-      <c r="R23" s="45"/>
-      <c r="X23" s="54"/>
-      <c r="Y23" s="54"/>
-      <c r="Z23" s="54"/>
-      <c r="AA23" s="54"/>
-      <c r="AB23" s="54"/>
-    </row>
-    <row r="24" spans="3:28">
-      <c r="C24" s="48" t="s">
+      <c r="P23" s="40"/>
+      <c r="Q23" s="40"/>
+      <c r="R23" s="40"/>
+      <c r="X23" s="27"/>
+      <c r="Y23" s="27"/>
+      <c r="Z23" s="27"/>
+      <c r="AA23" s="27"/>
+      <c r="AB23" s="27"/>
+    </row>
+    <row r="24" spans="2:28">
+      <c r="C24" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
       <c r="O24" s="19" t="s">
         <v>113</v>
       </c>
@@ -2027,7 +2046,7 @@
       </c>
       <c r="R24" s="20"/>
     </row>
-    <row r="25" spans="3:28">
+    <row r="25" spans="2:28">
       <c r="C25" s="20" t="s">
         <v>67</v>
       </c>
@@ -2048,11 +2067,11 @@
       </c>
       <c r="R25" s="20"/>
     </row>
-    <row r="26" spans="3:28">
+    <row r="26" spans="2:28">
       <c r="C26" s="20">
         <v>1</v>
       </c>
-      <c r="D26" s="49">
+      <c r="D26" s="24">
         <v>701</v>
       </c>
       <c r="E26" s="20" t="s">
@@ -2069,11 +2088,11 @@
       </c>
       <c r="R26" s="20"/>
     </row>
-    <row r="27" spans="3:28">
+    <row r="27" spans="2:28">
       <c r="C27" s="20">
         <v>2</v>
       </c>
-      <c r="D27" s="49">
+      <c r="D27" s="24">
         <v>701</v>
       </c>
       <c r="E27" s="20" t="s">
@@ -2090,11 +2109,11 @@
       </c>
       <c r="R27" s="20"/>
     </row>
-    <row r="28" spans="3:28">
+    <row r="28" spans="2:28">
       <c r="C28" s="20">
         <v>3</v>
       </c>
-      <c r="D28" s="49">
+      <c r="D28" s="24">
         <v>701</v>
       </c>
       <c r="E28" s="20" t="s">
@@ -2105,16 +2124,16 @@
       <c r="Q28" s="20"/>
       <c r="R28" s="20"/>
     </row>
-    <row r="30" spans="3:28" ht="26.25">
-      <c r="C30" s="34" t="s">
+    <row r="30" spans="2:28" ht="26.25">
+      <c r="C30" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="35"/>
+      <c r="D30" s="48"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="48"/>
+      <c r="I30" s="49"/>
       <c r="J30" s="12"/>
       <c r="K30" s="8"/>
       <c r="L30" s="8" t="s">
@@ -2124,7 +2143,7 @@
       <c r="N30" s="8"/>
       <c r="O30" s="8"/>
     </row>
-    <row r="31" spans="3:28">
+    <row r="31" spans="2:28">
       <c r="C31" s="10" t="s">
         <v>72</v>
       </c>
@@ -2171,7 +2190,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="3:28">
+    <row r="32" spans="2:28">
       <c r="C32" s="10">
         <v>1</v>
       </c>
@@ -2417,16 +2436,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="L15:M15"/>
     <mergeCell ref="O23:R23"/>
     <mergeCell ref="O15:R15"/>
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="X3:Y3"/>
     <mergeCell ref="X16:AB16"/>
-    <mergeCell ref="C30:I30"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="L15:M15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>